<commit_message>
Fix long path (260 chars path length)
</commit_message>
<xml_diff>
--- a/SetACLs/BlankTemplate.xlsx
+++ b/SetACLs/BlankTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DucHN3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DucHN3\Documents\Visual Studio 2015\Projects\SetACLs\SetACLs\bin\Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -420,12 +420,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -454,6 +448,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -684,85 +684,85 @@
   <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="5" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -771,101 +771,101 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="6" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="6" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -879,6 +879,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDDDDD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1437,22 +1442,22 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="55"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="54"/>
     </row>
     <row r="15" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="8"/>
@@ -1471,22 +1476,22 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="55"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="54"/>
     </row>
     <row r="17" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
@@ -1557,16 +1562,16 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58" t="s">
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="58"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
@@ -1577,16 +1582,16 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="62" t="s">
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="62"/>
-      <c r="K22" s="63"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="62"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -1597,16 +1602,16 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="51" t="s">
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="51"/>
-      <c r="K23" s="52"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -1838,18 +1843,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B3" s="17"/>
@@ -1881,17 +1886,17 @@
       <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="68"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B6" s="22"/>
@@ -1961,15 +1966,15 @@
     </row>
     <row r="11" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="70"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
@@ -2027,17 +2032,17 @@
     </row>
     <row r="16" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="26"/>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="68"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="75"/>
     </row>
     <row r="17" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
@@ -2069,69 +2074,69 @@
     </row>
     <row r="19" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B19" s="21"/>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="74"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="68"/>
     </row>
     <row r="20" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
     </row>
     <row r="21" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="26"/>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="68"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="75"/>
     </row>
     <row r="22" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="26"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="68"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="75"/>
     </row>
     <row r="23" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="26"/>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="68"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
     </row>
     <row r="24" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B24" s="26"/>
@@ -2149,73 +2154,73 @@
     </row>
     <row r="25" spans="2:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="26"/>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="70"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="26"/>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="70"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="26"/>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="70"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="66"/>
     </row>
     <row r="28" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="27"/>
-      <c r="C28" s="71" t="s">
+      <c r="C28" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C28:K28"/>
-    <mergeCell ref="C27:K27"/>
-    <mergeCell ref="C19:K20"/>
-    <mergeCell ref="C26:K26"/>
-    <mergeCell ref="C11:K11"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C16:K16"/>
     <mergeCell ref="C23:K23"/>
     <mergeCell ref="C25:K25"/>
     <mergeCell ref="C5:K5"/>
     <mergeCell ref="C21:K22"/>
+    <mergeCell ref="C28:K28"/>
+    <mergeCell ref="C27:K27"/>
+    <mergeCell ref="C19:K20"/>
+    <mergeCell ref="C26:K26"/>
+    <mergeCell ref="C11:K11"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2227,7 +2232,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2255,15 +2260,15 @@
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.15">
-      <c r="A3" s="48"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="46"/>
       <c r="D3"/>
       <c r="E3"/>

</xml_diff>